<commit_message>
doesn't work when deployed - cannot store data within functionapp. need to implement BytesIO algorithm works! beta version. maybe some .wav normalisation?
Signed-off-by: crushyna <crushyna@gmail.com>
</commit_message>
<xml_diff>
--- a/resultbook.xlsx
+++ b/resultbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crushyna\PycharmProjects\biometrical_speaker_recognizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD156649-DEA2-4BC6-B48E-BE2F1B88789A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FAE47DD-87D4-4862-B6F1-7A564876A948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20052" yWindow="-396" windowWidth="23256" windowHeight="13176" xr2:uid="{D0780C45-68DF-4347-95AB-5CC5FC63E0FC}"/>
   </bookViews>
@@ -323,14 +323,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -651,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35BB396A-6F11-46F0-8F26-6E7FC33E3E33}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,14 +664,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -703,10 +703,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
+      <c r="A3" s="21">
         <v>1</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -732,8 +732,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
@@ -757,10 +757,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="22">
+      <c r="A5" s="21">
         <v>2</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -786,8 +786,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="22"/>
-      <c r="B6" s="23"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
@@ -811,10 +811,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
+      <c r="A7" s="21">
         <v>3</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="22" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -840,8 +840,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="6" t="s">
         <v>10</v>
       </c>
@@ -865,10 +865,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
+      <c r="A9" s="21">
         <v>4</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -894,8 +894,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="6" t="s">
         <v>10</v>
       </c>
@@ -919,10 +919,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
+      <c r="A11" s="21">
         <v>5</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -948,8 +948,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="23"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="6" t="s">
         <v>10</v>
       </c>
@@ -973,10 +973,10 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="22">
+      <c r="A13" s="21">
         <v>6</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1002,8 +1002,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="6" t="s">
         <v>10</v>
       </c>
@@ -1027,10 +1027,10 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="22">
+      <c r="A15" s="21">
         <v>7</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1056,8 +1056,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="6" t="s">
         <v>10</v>
       </c>
@@ -1081,10 +1081,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="22">
+      <c r="A17" s="21">
         <v>8</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="22" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -1110,8 +1110,8 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="6" t="s">
         <v>10</v>
       </c>
@@ -1135,10 +1135,10 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="22">
+      <c r="A19" s="21">
         <v>9</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="22" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -1164,8 +1164,8 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="23"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="22"/>
       <c r="C20" s="6" t="s">
         <v>10</v>
       </c>
@@ -1189,10 +1189,10 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="22">
+      <c r="A21" s="21">
         <v>10</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1218,8 +1218,8 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="22"/>
       <c r="C22" s="6" t="s">
         <v>10</v>
       </c>
@@ -1243,10 +1243,10 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="22">
+      <c r="A23" s="21">
         <v>11</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1272,8 +1272,8 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="23"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="22"/>
       <c r="C24" s="6" t="s">
         <v>10</v>
       </c>
@@ -1297,10 +1297,10 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="22">
+      <c r="A25" s="21">
         <v>12</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="22" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -1326,8 +1326,8 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
-      <c r="B26" s="23"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="22"/>
       <c r="C26" s="6" t="s">
         <v>10</v>
       </c>
@@ -1352,6 +1352,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B23:B24"/>
@@ -1368,15 +1377,6 @@
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A19:A20"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:I26">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
works correctly on local machine and online! needs auto voice array uploader implemented later maybe some .wav normalisation?
Signed-off-by: crushyna <crushyna@gmail.com>
</commit_message>
<xml_diff>
--- a/resultbook.xlsx
+++ b/resultbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crushyna\PycharmProjects\biometrical_speaker_recognizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FAE47DD-87D4-4862-B6F1-7A564876A948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB9819B-98C8-4918-8586-34C9A0E5B55E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20052" yWindow="-396" windowWidth="23256" windowHeight="13176" xr2:uid="{D0780C45-68DF-4347-95AB-5CC5FC63E0FC}"/>
+    <workbookView xWindow="1410" yWindow="1380" windowWidth="18900" windowHeight="11505" xr2:uid="{D0780C45-68DF-4347-95AB-5CC5FC63E0FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -323,14 +323,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -651,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35BB396A-6F11-46F0-8F26-6E7FC33E3E33}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,14 +664,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -703,10 +703,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="21">
+      <c r="A3" s="22">
         <v>1</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="23" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -732,8 +732,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
@@ -757,10 +757,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
+      <c r="A5" s="22">
         <v>2</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="23" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -786,8 +786,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
@@ -811,10 +811,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="21">
+      <c r="A7" s="22">
         <v>3</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="23" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -840,8 +840,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="22"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="6" t="s">
         <v>10</v>
       </c>
@@ -865,10 +865,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="21">
+      <c r="A9" s="22">
         <v>4</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="23" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -894,8 +894,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
-      <c r="B10" s="22"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="6" t="s">
         <v>10</v>
       </c>
@@ -919,10 +919,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
+      <c r="A11" s="22">
         <v>5</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="23" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -948,8 +948,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="22"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="6" t="s">
         <v>10</v>
       </c>
@@ -973,10 +973,10 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="21">
+      <c r="A13" s="22">
         <v>6</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="23" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1002,8 +1002,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21"/>
-      <c r="B14" s="22"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="6" t="s">
         <v>10</v>
       </c>
@@ -1027,10 +1027,10 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="21">
+      <c r="A15" s="22">
         <v>7</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="23" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1056,8 +1056,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="22"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="6" t="s">
         <v>10</v>
       </c>
@@ -1081,10 +1081,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
+      <c r="A17" s="22">
         <v>8</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="23" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -1110,8 +1110,8 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="21"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="6" t="s">
         <v>10</v>
       </c>
@@ -1135,10 +1135,10 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="21">
+      <c r="A19" s="22">
         <v>9</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="23" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -1164,8 +1164,8 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="22"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="6" t="s">
         <v>10</v>
       </c>
@@ -1189,10 +1189,10 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="21">
+      <c r="A21" s="22">
         <v>10</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="23" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1218,8 +1218,8 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="21"/>
-      <c r="B22" s="22"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="6" t="s">
         <v>10</v>
       </c>
@@ -1243,10 +1243,10 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="21">
+      <c r="A23" s="22">
         <v>11</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="23" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1272,8 +1272,8 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="22"/>
+      <c r="A24" s="22"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="6" t="s">
         <v>10</v>
       </c>
@@ -1297,10 +1297,10 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="21">
+      <c r="A25" s="22">
         <v>12</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -1326,8 +1326,8 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="21"/>
-      <c r="B26" s="22"/>
+      <c r="A26" s="22"/>
+      <c r="B26" s="23"/>
       <c r="C26" s="6" t="s">
         <v>10</v>
       </c>
@@ -1352,15 +1352,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B23:B24"/>
@@ -1377,6 +1368,15 @@
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A19:A20"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:I26">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
works on azure! updated for various texts! maybe some .wav normalisation?
Signed-off-by: crushyna <crushyna@gmail.com>
</commit_message>
<xml_diff>
--- a/resultbook.xlsx
+++ b/resultbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crushyna\PycharmProjects\biometrical_speaker_recognizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB9819B-98C8-4918-8586-34C9A0E5B55E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6313F7D-BA70-495A-9004-EA96FFBC36BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="1380" windowWidth="18900" windowHeight="11505" xr2:uid="{D0780C45-68DF-4347-95AB-5CC5FC63E0FC}"/>
+    <workbookView xWindow="870" yWindow="1140" windowWidth="18900" windowHeight="11310" xr2:uid="{D0780C45-68DF-4347-95AB-5CC5FC63E0FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -651,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35BB396A-6F11-46F0-8F26-6E7FC33E3E33}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
unused helpers - deleted maybe some .wav normalisation?
Signed-off-by: crushyna <crushyna@gmail.com>
</commit_message>
<xml_diff>
--- a/resultbook.xlsx
+++ b/resultbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crushyna\PycharmProjects\biometrical_speaker_recognizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6313F7D-BA70-495A-9004-EA96FFBC36BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DACB1E9-8D0E-49A9-93E4-679F2D02BB5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="870" yWindow="1140" windowWidth="18900" windowHeight="11310" xr2:uid="{D0780C45-68DF-4347-95AB-5CC5FC63E0FC}"/>
   </bookViews>
@@ -323,14 +323,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -651,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35BB396A-6F11-46F0-8F26-6E7FC33E3E33}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,14 +664,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -703,10 +703,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
+      <c r="A3" s="21">
         <v>1</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -732,8 +732,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
@@ -757,10 +757,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="22">
+      <c r="A5" s="21">
         <v>2</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -786,8 +786,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="22"/>
-      <c r="B6" s="23"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
@@ -811,10 +811,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
+      <c r="A7" s="21">
         <v>3</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="22" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -840,8 +840,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="6" t="s">
         <v>10</v>
       </c>
@@ -865,10 +865,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
+      <c r="A9" s="21">
         <v>4</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -894,8 +894,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="6" t="s">
         <v>10</v>
       </c>
@@ -919,10 +919,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
+      <c r="A11" s="21">
         <v>5</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -948,8 +948,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="23"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="6" t="s">
         <v>10</v>
       </c>
@@ -973,10 +973,10 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="22">
+      <c r="A13" s="21">
         <v>6</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1002,8 +1002,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="6" t="s">
         <v>10</v>
       </c>
@@ -1027,10 +1027,10 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="22">
+      <c r="A15" s="21">
         <v>7</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1056,8 +1056,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="6" t="s">
         <v>10</v>
       </c>
@@ -1081,10 +1081,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="22">
+      <c r="A17" s="21">
         <v>8</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="22" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -1110,8 +1110,8 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="6" t="s">
         <v>10</v>
       </c>
@@ -1135,10 +1135,10 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="22">
+      <c r="A19" s="21">
         <v>9</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="22" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -1164,8 +1164,8 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="23"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="22"/>
       <c r="C20" s="6" t="s">
         <v>10</v>
       </c>
@@ -1189,10 +1189,10 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="22">
+      <c r="A21" s="21">
         <v>10</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1218,8 +1218,8 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="22"/>
       <c r="C22" s="6" t="s">
         <v>10</v>
       </c>
@@ -1243,10 +1243,10 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="22">
+      <c r="A23" s="21">
         <v>11</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1272,8 +1272,8 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="23"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="22"/>
       <c r="C24" s="6" t="s">
         <v>10</v>
       </c>
@@ -1297,10 +1297,10 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="22">
+      <c r="A25" s="21">
         <v>12</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="22" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -1326,8 +1326,8 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
-      <c r="B26" s="23"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="22"/>
       <c r="C26" s="6" t="s">
         <v>10</v>
       </c>
@@ -1352,6 +1352,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B23:B24"/>
@@ -1368,15 +1377,6 @@
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A19:A20"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:I26">
     <cfRule type="colorScale" priority="1">

</xml_diff>